<commit_message>
add eda and change order
</commit_message>
<xml_diff>
--- a/socks_current_data.xlsx
+++ b/socks_current_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -451,7 +451,7 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>price</t>
+          <t>price_in_PLN</t>
         </is>
       </c>
     </row>
@@ -473,7 +473,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>49.95 zł</t>
+          <t>49.95</t>
         </is>
       </c>
     </row>
@@ -495,7 +495,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>49.95 zł</t>
+          <t>49.95</t>
         </is>
       </c>
     </row>
@@ -517,7 +517,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>49.95 zł</t>
+          <t>49.95</t>
         </is>
       </c>
     </row>
@@ -534,12 +534,12 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>royal blue</t>
+          <t>blue</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>49.95 zł</t>
+          <t>49.95</t>
         </is>
       </c>
     </row>
@@ -561,7 +561,7 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>49.95 zł</t>
+          <t>49.95</t>
         </is>
       </c>
     </row>
@@ -578,12 +578,12 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>maroon</t>
+          <t>burgundy</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>49.95 zł</t>
+          <t>49.95</t>
         </is>
       </c>
     </row>
@@ -595,17 +595,17 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>IB7822</t>
+          <t>IB7821</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>light blue</t>
+          <t>orange</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>49.95 zł</t>
+          <t>49.95</t>
         </is>
       </c>
     </row>
@@ -617,17 +617,17 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>IB7823</t>
+          <t>IB7822</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>mint</t>
+          <t>blue</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>49.95 zł</t>
+          <t>49.95</t>
         </is>
       </c>
     </row>
@@ -639,17 +639,17 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>IB7821</t>
+          <t>IB7823</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>orange</t>
+          <t>mint</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>49.95 zł</t>
+          <t>49.95</t>
         </is>
       </c>
     </row>
@@ -671,7 +671,7 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>49.95 zł</t>
+          <t>49.95</t>
         </is>
       </c>
     </row>
@@ -688,12 +688,34 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>black</t>
+          <t>grey</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>49.95 zł</t>
+          <t>49.95</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>socks</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>IB7813</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>white</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>49.95</t>
         </is>
       </c>
     </row>

</xml_diff>